<commit_message>
feat: new PDF's to read
</commit_message>
<xml_diff>
--- a/Open-LPs.xlsx
+++ b/Open-LPs.xlsx
@@ -1,29 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27328"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mao8ct\Desktop\PyAutomateSAP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7871E331-DA03-48C8-9FF4-D196778528D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49500584-84B4-464C-A339-A7B64BD68979}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="19">
-  <si>
-    <t>Unnamed: 0</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>LP</t>
   </si>
@@ -31,52 +28,85 @@
     <t>Status</t>
   </si>
   <si>
-    <t>LP-044206</t>
-  </si>
-  <si>
-    <t>Encerrado!</t>
-  </si>
-  <si>
-    <t>LP-044240</t>
-  </si>
-  <si>
-    <t>LP-044242</t>
-  </si>
-  <si>
-    <t>LP-044459</t>
-  </si>
-  <si>
-    <t>LP-044460</t>
-  </si>
-  <si>
-    <t>LP-045063</t>
-  </si>
-  <si>
-    <t>LP-045227</t>
-  </si>
-  <si>
-    <t>LP-045395</t>
-  </si>
-  <si>
-    <t>LP-045593</t>
-  </si>
-  <si>
-    <t>LP-045774</t>
-  </si>
-  <si>
-    <t>LP-045794</t>
-  </si>
-  <si>
-    <t>Compromisso pendente!</t>
-  </si>
-  <si>
-    <t>LP-045965</t>
-  </si>
-  <si>
-    <t>LP-045988</t>
-  </si>
-  <si>
-    <t>LP-046278</t>
+    <t>LP-042681</t>
+  </si>
+  <si>
+    <t>LP-043967</t>
+  </si>
+  <si>
+    <t>LP-044159</t>
+  </si>
+  <si>
+    <t>LP-044184</t>
+  </si>
+  <si>
+    <t>LP-044484</t>
+  </si>
+  <si>
+    <t>LP-045246</t>
+  </si>
+  <si>
+    <t>LP-045247</t>
+  </si>
+  <si>
+    <t>LP-045255</t>
+  </si>
+  <si>
+    <t>LP-045283</t>
+  </si>
+  <si>
+    <t>LP-045323</t>
+  </si>
+  <si>
+    <t>LP-045325</t>
+  </si>
+  <si>
+    <t>LP-045341</t>
+  </si>
+  <si>
+    <t>LP-045504</t>
+  </si>
+  <si>
+    <t>LP-045506</t>
+  </si>
+  <si>
+    <t>LP-045507</t>
+  </si>
+  <si>
+    <t>LP-045510</t>
+  </si>
+  <si>
+    <t>LP-045511</t>
+  </si>
+  <si>
+    <t>LP-045368</t>
+  </si>
+  <si>
+    <t>LP-045812</t>
+  </si>
+  <si>
+    <t>LP-045817</t>
+  </si>
+  <si>
+    <t>LP-045904</t>
+  </si>
+  <si>
+    <t>LP-046049</t>
+  </si>
+  <si>
+    <t>LP-046050</t>
+  </si>
+  <si>
+    <t>LP-046055</t>
+  </si>
+  <si>
+    <t>LP-046639</t>
+  </si>
+  <si>
+    <t>LP-046640</t>
+  </si>
+  <si>
+    <t>LP-045940</t>
   </si>
 </sst>
 </file>
@@ -94,7 +124,10 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -155,9 +188,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -195,7 +228,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -229,6 +262,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -263,9 +297,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -439,184 +474,242 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
         <v>5</v>
       </c>
-      <c r="C3" t="s">
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="B6" t="s">
         <v>6</v>
       </c>
-      <c r="C4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
         <v>7</v>
       </c>
-      <c r="C5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
         <v>8</v>
       </c>
-      <c r="C6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
         <v>9</v>
       </c>
-      <c r="C7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
         <v>10</v>
       </c>
-      <c r="C8" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
         <v>11</v>
       </c>
-      <c r="C9" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>8</v>
-      </c>
-      <c r="B10" t="s">
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
         <v>12</v>
       </c>
-      <c r="C10" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>9</v>
-      </c>
-      <c r="B11" t="s">
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
         <v>13</v>
       </c>
-      <c r="C11" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>10</v>
-      </c>
-      <c r="B12" t="s">
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
         <v>14</v>
       </c>
-      <c r="C12" t="s">
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>11</v>
-      </c>
-      <c r="B13" t="s">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
         <v>16</v>
       </c>
-      <c r="C13" t="s">
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
         <v>15</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>12</v>
-      </c>
-      <c r="B14" t="s">
+      <c r="B17" t="s">
         <v>17</v>
       </c>
-      <c r="C14" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>13</v>
-      </c>
-      <c r="B15" t="s">
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
         <v>18</v>
       </c>
-      <c r="C15" t="s">
-        <v>4</v>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>23</v>
+      </c>
+      <c r="B25" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>24</v>
+      </c>
+      <c r="B26" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>25</v>
+      </c>
+      <c r="B27" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>26</v>
+      </c>
+      <c r="B28" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
attempt to fix: not finished yet
</commit_message>
<xml_diff>
--- a/Open-LPs.xlsx
+++ b/Open-LPs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mao8ct\Desktop\PyAutomateSAP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49500584-84B4-464C-A339-A7B64BD68979}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7071CAE3-180D-44F3-8ECE-37ABAF8A251C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>LP</t>
   </si>
@@ -28,85 +28,7 @@
     <t>Status</t>
   </si>
   <si>
-    <t>LP-042681</t>
-  </si>
-  <si>
-    <t>LP-043967</t>
-  </si>
-  <si>
-    <t>LP-044159</t>
-  </si>
-  <si>
-    <t>LP-044184</t>
-  </si>
-  <si>
-    <t>LP-044484</t>
-  </si>
-  <si>
-    <t>LP-045246</t>
-  </si>
-  <si>
-    <t>LP-045247</t>
-  </si>
-  <si>
-    <t>LP-045255</t>
-  </si>
-  <si>
-    <t>LP-045283</t>
-  </si>
-  <si>
-    <t>LP-045323</t>
-  </si>
-  <si>
-    <t>LP-045325</t>
-  </si>
-  <si>
-    <t>LP-045341</t>
-  </si>
-  <si>
-    <t>LP-045504</t>
-  </si>
-  <si>
-    <t>LP-045506</t>
-  </si>
-  <si>
-    <t>LP-045507</t>
-  </si>
-  <si>
-    <t>LP-045510</t>
-  </si>
-  <si>
-    <t>LP-045511</t>
-  </si>
-  <si>
-    <t>LP-045368</t>
-  </si>
-  <si>
-    <t>LP-045812</t>
-  </si>
-  <si>
-    <t>LP-045817</t>
-  </si>
-  <si>
-    <t>LP-045904</t>
-  </si>
-  <si>
-    <t>LP-046049</t>
-  </si>
-  <si>
-    <t>LP-046050</t>
-  </si>
-  <si>
-    <t>LP-046055</t>
-  </si>
-  <si>
-    <t>LP-046639</t>
-  </si>
-  <si>
-    <t>LP-046640</t>
-  </si>
-  <si>
-    <t>LP-045940</t>
+    <t>LP-046189</t>
   </si>
 </sst>
 </file>
@@ -165,9 +87,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -477,7 +402,7 @@
   <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -502,212 +427,82 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
+      <c r="A3" s="2"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
+      <c r="A4" s="2"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
+      <c r="A5" s="2"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>6</v>
-      </c>
+      <c r="A6" s="2"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
-        <v>7</v>
-      </c>
+      <c r="A7" s="2"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
-        <v>8</v>
-      </c>
+      <c r="A8" s="2"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
-        <v>9</v>
-      </c>
+      <c r="A9" s="2"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>8</v>
-      </c>
-      <c r="B10" t="s">
-        <v>10</v>
-      </c>
+      <c r="A10" s="2"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>9</v>
-      </c>
-      <c r="B11" t="s">
-        <v>11</v>
-      </c>
+      <c r="A11" s="2"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>10</v>
-      </c>
-      <c r="B12" t="s">
-        <v>12</v>
-      </c>
+      <c r="A12" s="2"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>11</v>
-      </c>
-      <c r="B13" t="s">
-        <v>13</v>
-      </c>
+      <c r="A13" s="2"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>12</v>
-      </c>
-      <c r="B14" t="s">
-        <v>14</v>
-      </c>
+      <c r="A14" s="2"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
-        <v>13</v>
-      </c>
-      <c r="B15" t="s">
-        <v>15</v>
-      </c>
+      <c r="A15" s="2"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
-        <v>14</v>
-      </c>
-      <c r="B16" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
-        <v>15</v>
-      </c>
-      <c r="B17" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
-        <v>16</v>
-      </c>
-      <c r="B18" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
-        <v>17</v>
-      </c>
-      <c r="B19" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
-        <v>18</v>
-      </c>
-      <c r="B20" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
-        <v>19</v>
-      </c>
-      <c r="B21" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
-        <v>20</v>
-      </c>
-      <c r="B22" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="1">
-        <v>21</v>
-      </c>
-      <c r="B23" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="1">
-        <v>22</v>
-      </c>
-      <c r="B24" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="1">
-        <v>23</v>
-      </c>
-      <c r="B25" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="1">
-        <v>24</v>
-      </c>
-      <c r="B26" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="1">
-        <v>25</v>
-      </c>
-      <c r="B27" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="1">
-        <v>26</v>
-      </c>
-      <c r="B28" t="s">
-        <v>27</v>
-      </c>
+      <c r="A16" s="2"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="2"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="2"/>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="2"/>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="2"/>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="2"/>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="2"/>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="2"/>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="2"/>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="2"/>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="2"/>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="2"/>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
used: bot to finish LPs
</commit_message>
<xml_diff>
--- a/Open-LPs.xlsx
+++ b/Open-LPs.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C61"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,7 +456,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>LP-039665</t>
+          <t>LP-038957</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -471,7 +471,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>LP-039679</t>
+          <t>LP-041062</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -486,7 +486,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>LP-039802</t>
+          <t>LP-041602</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -501,7 +501,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>LP-041458</t>
+          <t>LP-043674</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -516,7 +516,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>LP-043707</t>
+          <t>LP-044939</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -531,7 +531,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>LP-043894</t>
+          <t>LP-045263</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -546,7 +546,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>LP-044708</t>
+          <t>LP-045544</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -561,7 +561,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>LP-044750</t>
+          <t>LP-045688</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -576,7 +576,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>LP-044805</t>
+          <t>LP-046075</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -591,7 +591,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>LP-044836</t>
+          <t>LP-046351</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -606,7 +606,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>LP-045487</t>
+          <t>LP-046632</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -621,7 +621,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>LP-045489</t>
+          <t>LP-046666</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -636,12 +636,12 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>LP-045834</t>
+          <t>LP-046672</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Encerrado!</t>
+          <t>Compromisso pendente!</t>
         </is>
       </c>
     </row>
@@ -651,7 +651,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>LP-045875</t>
+          <t>LP-046943</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -666,12 +666,12 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>LP-045914</t>
+          <t>LP-046947</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Possui linhas de compra e apontamento!</t>
+          <t>Encerrado!</t>
         </is>
       </c>
     </row>
@@ -681,7 +681,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>LP-045933</t>
+          <t>LP-046949</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -696,7 +696,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>LP-045943</t>
+          <t>LP-046950</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -711,7 +711,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>LP-045972</t>
+          <t>LP-046954</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -726,7 +726,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>LP-046008</t>
+          <t>LP-047178</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -741,7 +741,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>LP-046035</t>
+          <t>LP-047180</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -756,7 +756,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>LP-046073</t>
+          <t>LP-047196</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -771,7 +771,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>LP-046236</t>
+          <t>LP-047514</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -779,436 +779,6 @@
           <t>Encerrado!</t>
         </is>
       </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="n">
-        <v>22</v>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>LP-046405</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>Encerrado!</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="n">
-        <v>23</v>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>LP-046411</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>Encerrado!</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="n">
-        <v>24</v>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>LP-046434</t>
-        </is>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>Encerrado!</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="n">
-        <v>25</v>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>LP-046435</t>
-        </is>
-      </c>
-      <c r="C27" t="inlineStr"/>
-    </row>
-    <row r="28">
-      <c r="A28" t="n">
-        <v>26</v>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>LP-046460</t>
-        </is>
-      </c>
-      <c r="C28" t="inlineStr"/>
-    </row>
-    <row r="29">
-      <c r="A29" t="n">
-        <v>27</v>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>LP-046461</t>
-        </is>
-      </c>
-      <c r="C29" t="inlineStr"/>
-    </row>
-    <row r="30">
-      <c r="A30" t="n">
-        <v>28</v>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>LP-046464</t>
-        </is>
-      </c>
-      <c r="C30" t="inlineStr"/>
-    </row>
-    <row r="31">
-      <c r="A31" t="n">
-        <v>29</v>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>LP-046468</t>
-        </is>
-      </c>
-      <c r="C31" t="inlineStr"/>
-    </row>
-    <row r="32">
-      <c r="A32" t="n">
-        <v>30</v>
-      </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>LP-046573</t>
-        </is>
-      </c>
-      <c r="C32" t="inlineStr"/>
-    </row>
-    <row r="33">
-      <c r="A33" t="n">
-        <v>31</v>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>LP-046637</t>
-        </is>
-      </c>
-      <c r="C33" t="inlineStr"/>
-    </row>
-    <row r="34">
-      <c r="A34" t="n">
-        <v>32</v>
-      </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>LP-046645</t>
-        </is>
-      </c>
-      <c r="C34" t="inlineStr"/>
-    </row>
-    <row r="35">
-      <c r="A35" t="n">
-        <v>33</v>
-      </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>LP-046850</t>
-        </is>
-      </c>
-      <c r="C35" t="inlineStr"/>
-    </row>
-    <row r="36">
-      <c r="A36" t="n">
-        <v>34</v>
-      </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>LP-046853</t>
-        </is>
-      </c>
-      <c r="C36" t="inlineStr"/>
-    </row>
-    <row r="37">
-      <c r="A37" t="n">
-        <v>35</v>
-      </c>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t>LP-046872</t>
-        </is>
-      </c>
-      <c r="C37" t="inlineStr"/>
-    </row>
-    <row r="38">
-      <c r="A38" t="n">
-        <v>36</v>
-      </c>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>LP-046873</t>
-        </is>
-      </c>
-      <c r="C38" t="inlineStr"/>
-    </row>
-    <row r="39">
-      <c r="A39" t="n">
-        <v>37</v>
-      </c>
-      <c r="B39" t="inlineStr">
-        <is>
-          <t>LP-046876</t>
-        </is>
-      </c>
-      <c r="C39" t="inlineStr"/>
-    </row>
-    <row r="40">
-      <c r="A40" t="n">
-        <v>38</v>
-      </c>
-      <c r="B40" t="inlineStr">
-        <is>
-          <t>LP-046878</t>
-        </is>
-      </c>
-      <c r="C40" t="inlineStr"/>
-    </row>
-    <row r="41">
-      <c r="A41" t="n">
-        <v>39</v>
-      </c>
-      <c r="B41" t="inlineStr">
-        <is>
-          <t>LP-046897</t>
-        </is>
-      </c>
-      <c r="C41" t="inlineStr"/>
-    </row>
-    <row r="42">
-      <c r="A42" t="n">
-        <v>40</v>
-      </c>
-      <c r="B42" t="inlineStr">
-        <is>
-          <t>LP-046898</t>
-        </is>
-      </c>
-      <c r="C42" t="inlineStr"/>
-    </row>
-    <row r="43">
-      <c r="A43" t="n">
-        <v>41</v>
-      </c>
-      <c r="B43" t="inlineStr">
-        <is>
-          <t>LP-046911</t>
-        </is>
-      </c>
-      <c r="C43" t="inlineStr"/>
-    </row>
-    <row r="44">
-      <c r="A44" t="n">
-        <v>42</v>
-      </c>
-      <c r="B44" t="inlineStr">
-        <is>
-          <t>LP-046912</t>
-        </is>
-      </c>
-      <c r="C44" t="inlineStr"/>
-    </row>
-    <row r="45">
-      <c r="A45" t="n">
-        <v>43</v>
-      </c>
-      <c r="B45" t="inlineStr">
-        <is>
-          <t>LP-047048</t>
-        </is>
-      </c>
-      <c r="C45" t="inlineStr"/>
-    </row>
-    <row r="46">
-      <c r="A46" t="n">
-        <v>44</v>
-      </c>
-      <c r="B46" t="inlineStr">
-        <is>
-          <t>LP-047058</t>
-        </is>
-      </c>
-      <c r="C46" t="inlineStr"/>
-    </row>
-    <row r="47">
-      <c r="A47" t="n">
-        <v>45</v>
-      </c>
-      <c r="B47" t="inlineStr">
-        <is>
-          <t>LP-047149</t>
-        </is>
-      </c>
-      <c r="C47" t="inlineStr"/>
-    </row>
-    <row r="48">
-      <c r="A48" t="n">
-        <v>46</v>
-      </c>
-      <c r="B48" t="inlineStr">
-        <is>
-          <t>LP-047317</t>
-        </is>
-      </c>
-      <c r="C48" t="inlineStr"/>
-    </row>
-    <row r="49">
-      <c r="A49" t="n">
-        <v>47</v>
-      </c>
-      <c r="B49" t="inlineStr">
-        <is>
-          <t>LP-047368</t>
-        </is>
-      </c>
-      <c r="C49" t="inlineStr"/>
-    </row>
-    <row r="50">
-      <c r="A50" t="n">
-        <v>48</v>
-      </c>
-      <c r="B50" t="inlineStr">
-        <is>
-          <t>LP-047402</t>
-        </is>
-      </c>
-      <c r="C50" t="inlineStr"/>
-    </row>
-    <row r="51">
-      <c r="A51" t="n">
-        <v>49</v>
-      </c>
-      <c r="B51" t="inlineStr">
-        <is>
-          <t>LP-047450</t>
-        </is>
-      </c>
-      <c r="C51" t="inlineStr"/>
-    </row>
-    <row r="52">
-      <c r="A52" t="n">
-        <v>50</v>
-      </c>
-      <c r="B52" t="inlineStr">
-        <is>
-          <t>LP-047567</t>
-        </is>
-      </c>
-      <c r="C52" t="inlineStr"/>
-    </row>
-    <row r="53">
-      <c r="A53" t="n">
-        <v>51</v>
-      </c>
-      <c r="B53" t="inlineStr">
-        <is>
-          <t>LP-047722</t>
-        </is>
-      </c>
-      <c r="C53" t="inlineStr"/>
-    </row>
-    <row r="54">
-      <c r="A54" t="n">
-        <v>52</v>
-      </c>
-      <c r="B54" t="inlineStr">
-        <is>
-          <t>LP-047779</t>
-        </is>
-      </c>
-      <c r="C54" t="inlineStr"/>
-    </row>
-    <row r="55">
-      <c r="A55" t="n">
-        <v>53</v>
-      </c>
-      <c r="B55" t="inlineStr">
-        <is>
-          <t>LP-047811</t>
-        </is>
-      </c>
-      <c r="C55" t="inlineStr"/>
-    </row>
-    <row r="56">
-      <c r="A56" t="n">
-        <v>54</v>
-      </c>
-      <c r="B56" t="inlineStr">
-        <is>
-          <t>LP-047817</t>
-        </is>
-      </c>
-      <c r="C56" t="inlineStr"/>
-    </row>
-    <row r="57">
-      <c r="A57" t="n">
-        <v>55</v>
-      </c>
-      <c r="B57" t="inlineStr">
-        <is>
-          <t>LP-047906</t>
-        </is>
-      </c>
-      <c r="C57" t="inlineStr"/>
-    </row>
-    <row r="58">
-      <c r="A58" t="n">
-        <v>56</v>
-      </c>
-      <c r="B58" t="inlineStr">
-        <is>
-          <t>LP-047929</t>
-        </is>
-      </c>
-      <c r="C58" t="inlineStr"/>
-    </row>
-    <row r="59">
-      <c r="A59" t="n">
-        <v>57</v>
-      </c>
-      <c r="B59" t="inlineStr">
-        <is>
-          <t>LP-047942</t>
-        </is>
-      </c>
-      <c r="C59" t="inlineStr"/>
-    </row>
-    <row r="60">
-      <c r="A60" t="n">
-        <v>58</v>
-      </c>
-      <c r="B60" t="inlineStr">
-        <is>
-          <t>LP-047016</t>
-        </is>
-      </c>
-      <c r="C60" t="inlineStr"/>
-    </row>
-    <row r="61">
-      <c r="A61" t="n">
-        <v>59</v>
-      </c>
-      <c r="B61" t="inlineStr">
-        <is>
-          <t>LP-047119</t>
-        </is>
-      </c>
-      <c r="C61" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
feat: new KW PDF's added and bot finish-LP updated
</commit_message>
<xml_diff>
--- a/Open-LPs.xlsx
+++ b/Open-LPs.xlsx
@@ -1,66 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mao8ct\Desktop\PyAutomateSAP\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0363F795-3D85-4859-97A3-9FA1E0892E43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
-  <si>
-    <t>LP</t>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>LP-043866</t>
-  </si>
-  <si>
-    <t>Compromisso pendente!</t>
-  </si>
-  <si>
-    <t>LP-047940</t>
-  </si>
-  <si>
-    <t>LP-048445</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -75,43 +46,93 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -399,49 +420,305 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.42578125" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>3</v>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>LP</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Status</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>LP-111841</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Encerrado!</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>LP-048623</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Encerrado!</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>LP-048299</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Encerrado!</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>LP-048286</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Encerrado!</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>LP-048203</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Encerrado!</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>LP-046987</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Encerrado!</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>LP-048905</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Encerrado!</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>LP-110505</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Encerrado!</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>LP-048084</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Encerrado!</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>LP-047390</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Encerrado!</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>LP-047391</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Encerrado!</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>LP-048400</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Encerrado!</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>LP-048401</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Encerrado!</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>LP-048280</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Encerrado!</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>LP-113048</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Encerrado!</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>LP-048632</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Encerrado!</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>LP-048959</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Encerrado!</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>LP-048826</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Encerrado!</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>LP-048625</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Encerrado!</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>LP-048627</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Encerrado!</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>LP-113069</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Encerrado!</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>LP-111952</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>LP não existe!</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>LP-113071</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Encerrado!</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
used: finish-LP bot used
</commit_message>
<xml_diff>
--- a/Open-LPs.xlsx
+++ b/Open-LPs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mao8ct\Desktop\PyAutomateSAP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC50AF89-EA25-47E9-B005-E4943C0FA2EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D54B7C3A-813E-4C46-8AF0-C691A1F7E96B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,132 +20,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>LP</t>
   </si>
   <si>
     <t>Status</t>
-  </si>
-  <si>
-    <t>LP-043681</t>
-  </si>
-  <si>
-    <t>LP-043683</t>
-  </si>
-  <si>
-    <t>LP-045106</t>
-  </si>
-  <si>
-    <t>LP-045221</t>
-  </si>
-  <si>
-    <t>LP-047165</t>
-  </si>
-  <si>
-    <t>LP-047213</t>
-  </si>
-  <si>
-    <t>LP-047668</t>
-  </si>
-  <si>
-    <t>LP-047669</t>
-  </si>
-  <si>
-    <t>LP-047670</t>
-  </si>
-  <si>
-    <t>LP-047738</t>
-  </si>
-  <si>
-    <t>LP-047851</t>
-  </si>
-  <si>
-    <t>LP-048072</t>
-  </si>
-  <si>
-    <t>LP-048128</t>
-  </si>
-  <si>
-    <t>LP-048131</t>
-  </si>
-  <si>
-    <t>LP-048215</t>
-  </si>
-  <si>
-    <t>LP-048245</t>
-  </si>
-  <si>
-    <t>LP-048284</t>
-  </si>
-  <si>
-    <t>LP-048417</t>
-  </si>
-  <si>
-    <t>LP-048500</t>
-  </si>
-  <si>
-    <t>LP-048837</t>
-  </si>
-  <si>
-    <t>LP-048911</t>
-  </si>
-  <si>
-    <t>LP-049111</t>
-  </si>
-  <si>
-    <t>LP-049270</t>
-  </si>
-  <si>
-    <t>LP-049308</t>
-  </si>
-  <si>
-    <t>LP-049560</t>
-  </si>
-  <si>
-    <t>LP-049566</t>
-  </si>
-  <si>
-    <t>LP-049589</t>
-  </si>
-  <si>
-    <t>LP-049591</t>
-  </si>
-  <si>
-    <t>LP-049593</t>
-  </si>
-  <si>
-    <t>LP-049632</t>
-  </si>
-  <si>
-    <t>LP-049633</t>
-  </si>
-  <si>
-    <t>LP-049753</t>
-  </si>
-  <si>
-    <t>LP-033830</t>
-  </si>
-  <si>
-    <t>LP-046084</t>
-  </si>
-  <si>
-    <t>LP-046162</t>
-  </si>
-  <si>
-    <t>LP-046172</t>
-  </si>
-  <si>
-    <t>LP-046232</t>
-  </si>
-  <si>
-    <t>LP-046339</t>
-  </si>
-  <si>
-    <t>LP-046350</t>
-  </si>
-  <si>
-    <t>LP-047095</t>
   </si>
   <si>
     <t>LP-047259</t>
@@ -571,15 +451,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B62"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.42578125" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -694,206 +572,6 @@
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>62</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>